<commit_message>
Archivo con el desarrollo del ejercicio
</commit_message>
<xml_diff>
--- a/Ejercicio de prueba/Resolución del ejercicio.xlsx
+++ b/Ejercicio de prueba/Resolución del ejercicio.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cinthyadiaz/Estadistica_II/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cinthyadiaz/Estadistica_II/Ejercicio de prueba/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="24960" windowHeight="14740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Planteamiento del modelo</t>
+  </si>
+  <si>
+    <t>Planteamiento de las hipótesis</t>
   </si>
 </sst>
 </file>
@@ -86,13 +89,13 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>419094</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:colOff>152393</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="13550905" cy="821451"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <xdr:ext cx="13855706" cy="821451"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1"/>
@@ -100,8 +103,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm rot="10800000" flipV="1">
-              <a:off x="1244594" y="977900"/>
-              <a:ext cx="13550905" cy="821451"/>
+              <a:off x="977893" y="749300"/>
+              <a:ext cx="13855706" cy="821451"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -123,33 +126,34 @@
             </a:fontRef>
           </xdr:style>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr">
               <a:noAutofit/>
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr algn="ctr"/>
               <a14:m>
                 <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:r>
-                    <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                    <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                       <a:latin typeface="Cambria Math" charset="0"/>
                     </a:rPr>
                     <m:t>𝑃</m:t>
                   </m:r>
                   <m:r>
-                    <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                    <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                       <a:latin typeface="Cambria Math" charset="0"/>
                     </a:rPr>
                     <m:t>(</m:t>
                   </m:r>
                   <m:r>
-                    <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                    <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                       <a:latin typeface="Cambria Math" charset="0"/>
                     </a:rPr>
                     <m:t>𝑉𝑜𝑡𝑜</m:t>
                   </m:r>
                   <m:r>
-                    <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                    <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                       <a:latin typeface="Cambria Math" charset="0"/>
                     </a:rPr>
                     <m:t>)=</m:t>
@@ -157,14 +161,14 @@
                   <m:f>
                     <m:fPr>
                       <m:ctrlPr>
-                        <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                        <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                           <a:latin typeface="Cambria Math" charset="0"/>
                         </a:rPr>
                       </m:ctrlPr>
                     </m:fPr>
                     <m:num>
                       <m:r>
-                        <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                        <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                           <a:latin typeface="Cambria Math" charset="0"/>
                         </a:rPr>
                         <m:t>1</m:t>
@@ -172,7 +176,7 @@
                     </m:num>
                     <m:den>
                       <m:r>
-                        <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                        <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                           <a:latin typeface="Cambria Math" charset="0"/>
                         </a:rPr>
                         <m:t>1+ </m:t>
@@ -180,14 +184,14 @@
                       <m:sSup>
                         <m:sSupPr>
                           <m:ctrlPr>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                           </m:ctrlPr>
                         </m:sSupPr>
                         <m:e>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>𝑒</m:t>
@@ -195,7 +199,7 @@
                         </m:e>
                         <m:sup>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>−(</m:t>
@@ -203,14 +207,14 @@
                           <m:sSub>
                             <m:sSubPr>
                               <m:ctrlPr>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                 </a:rPr>
                               </m:ctrlPr>
                             </m:sSubPr>
                             <m:e>
                               <m:r>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                   <a:ea typeface="Cambria Math" charset="0"/>
                                   <a:cs typeface="Cambria Math" charset="0"/>
@@ -220,7 +224,7 @@
                             </m:e>
                             <m:sub>
                               <m:r>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                 </a:rPr>
                                 <m:t>0</m:t>
@@ -228,7 +232,7 @@
                             </m:sub>
                           </m:sSub>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>+</m:t>
@@ -236,14 +240,14 @@
                           <m:sSub>
                             <m:sSubPr>
                               <m:ctrlPr>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                 </a:rPr>
                               </m:ctrlPr>
                             </m:sSubPr>
                             <m:e>
                               <m:r>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                   <a:ea typeface="Cambria Math" charset="0"/>
                                   <a:cs typeface="Cambria Math" charset="0"/>
@@ -253,7 +257,7 @@
                             </m:e>
                             <m:sub>
                               <m:r>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                 </a:rPr>
                                 <m:t>1</m:t>
@@ -261,13 +265,13 @@
                             </m:sub>
                           </m:sSub>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>𝐼𝑛𝑑𝑖𝑣𝑖𝑑𝑢𝑎𝑙𝑖𝑠𝑚𝑜</m:t>
                           </m:r>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>+</m:t>
@@ -275,14 +279,14 @@
                           <m:sSub>
                             <m:sSubPr>
                               <m:ctrlPr>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                 </a:rPr>
                               </m:ctrlPr>
                             </m:sSubPr>
                             <m:e>
                               <m:r>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                   <a:ea typeface="Cambria Math" charset="0"/>
                                   <a:cs typeface="Cambria Math" charset="0"/>
@@ -292,7 +296,7 @@
                             </m:e>
                             <m:sub>
                               <m:r>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                 </a:rPr>
                                 <m:t>2</m:t>
@@ -300,13 +304,13 @@
                             </m:sub>
                           </m:sSub>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>𝐸𝑑𝑎𝑑</m:t>
                           </m:r>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>+</m:t>
@@ -314,14 +318,14 @@
                           <m:sSub>
                             <m:sSubPr>
                               <m:ctrlPr>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                 </a:rPr>
                               </m:ctrlPr>
                             </m:sSubPr>
                             <m:e>
                               <m:r>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                   <a:ea typeface="Cambria Math" charset="0"/>
                                   <a:cs typeface="Cambria Math" charset="0"/>
@@ -331,7 +335,7 @@
                             </m:e>
                             <m:sub>
                               <m:r>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                 </a:rPr>
                                 <m:t>3</m:t>
@@ -339,13 +343,13 @@
                             </m:sub>
                           </m:sSub>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>𝑅𝑒𝑠𝑖𝑑𝑒𝑛𝑐𝑖𝑎</m:t>
                           </m:r>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>+ </m:t>
@@ -353,14 +357,14 @@
                           <m:sSub>
                             <m:sSubPr>
                               <m:ctrlPr>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                 </a:rPr>
                               </m:ctrlPr>
                             </m:sSubPr>
                             <m:e>
                               <m:r>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                   <a:ea typeface="Cambria Math" charset="0"/>
                                   <a:cs typeface="Cambria Math" charset="0"/>
@@ -370,7 +374,7 @@
                             </m:e>
                             <m:sub>
                               <m:r>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                 </a:rPr>
                                 <m:t>4</m:t>
@@ -378,13 +382,13 @@
                             </m:sub>
                           </m:sSub>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>𝑁𝑆𝐸</m:t>
                           </m:r>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>+</m:t>
@@ -392,14 +396,14 @@
                           <m:sSub>
                             <m:sSubPr>
                               <m:ctrlPr>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                 </a:rPr>
                               </m:ctrlPr>
                             </m:sSubPr>
                             <m:e>
                               <m:r>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                   <a:ea typeface="Cambria Math" charset="0"/>
                                   <a:cs typeface="Cambria Math" charset="0"/>
@@ -409,7 +413,7 @@
                             </m:e>
                             <m:sub>
                               <m:r>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                 </a:rPr>
                                 <m:t>5</m:t>
@@ -417,25 +421,25 @@
                             </m:sub>
                           </m:sSub>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>𝑃𝑟𝑖𝑚𝑒𝑟𝑎</m:t>
                           </m:r>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t> </m:t>
                           </m:r>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>𝑣𝑢𝑒𝑙𝑡𝑎</m:t>
                           </m:r>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>+</m:t>
@@ -443,14 +447,14 @@
                           <m:sSub>
                             <m:sSubPr>
                               <m:ctrlPr>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                 </a:rPr>
                               </m:ctrlPr>
                             </m:sSubPr>
                             <m:e>
                               <m:r>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                   <a:ea typeface="Cambria Math" charset="0"/>
                                   <a:cs typeface="Cambria Math" charset="0"/>
@@ -460,7 +464,7 @@
                             </m:e>
                             <m:sub>
                               <m:r>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                 </a:rPr>
                                 <m:t>6</m:t>
@@ -468,13 +472,13 @@
                             </m:sub>
                           </m:sSub>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>𝐴𝑐𝑡𝑖𝑣𝑖𝑑𝑎𝑑</m:t>
                           </m:r>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>+</m:t>
@@ -482,14 +486,14 @@
                           <m:sSub>
                             <m:sSubPr>
                               <m:ctrlPr>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                 </a:rPr>
                               </m:ctrlPr>
                             </m:sSubPr>
                             <m:e>
                               <m:r>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                   <a:ea typeface="Cambria Math" charset="0"/>
                                   <a:cs typeface="Cambria Math" charset="0"/>
@@ -499,7 +503,7 @@
                             </m:e>
                             <m:sub>
                               <m:r>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                 </a:rPr>
                                 <m:t>6</m:t>
@@ -507,37 +511,37 @@
                             </m:sub>
                           </m:sSub>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>𝑁𝑜</m:t>
                           </m:r>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t> </m:t>
                           </m:r>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>𝑎</m:t>
                           </m:r>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t> </m:t>
                           </m:r>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>𝐾𝑒𝑖𝑘𝑜</m:t>
                           </m:r>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>+</m:t>
@@ -545,14 +549,14 @@
                           <m:sSub>
                             <m:sSubPr>
                               <m:ctrlPr>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                 </a:rPr>
                               </m:ctrlPr>
                             </m:sSubPr>
                             <m:e>
                               <m:r>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                   <a:ea typeface="Cambria Math" charset="0"/>
                                   <a:cs typeface="Cambria Math" charset="0"/>
@@ -562,7 +566,7 @@
                             </m:e>
                             <m:sub>
                               <m:r>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                 </a:rPr>
                                 <m:t>7</m:t>
@@ -570,49 +574,49 @@
                             </m:sub>
                           </m:sSub>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>𝑀𝑖𝑡𝑖𝑛</m:t>
                           </m:r>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t> </m:t>
                           </m:r>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>𝑁𝑜</m:t>
                           </m:r>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t> </m:t>
                           </m:r>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>𝑎</m:t>
                           </m:r>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t> </m:t>
                           </m:r>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>𝑘𝑒𝑖𝑘𝑜</m:t>
                           </m:r>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>+</m:t>
@@ -620,14 +624,14 @@
                           <m:sSub>
                             <m:sSubPr>
                               <m:ctrlPr>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                 </a:rPr>
                               </m:ctrlPr>
                             </m:sSubPr>
                             <m:e>
                               <m:r>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                   <a:ea typeface="Cambria Math" charset="0"/>
                                   <a:cs typeface="Cambria Math" charset="0"/>
@@ -637,7 +641,7 @@
                             </m:e>
                             <m:sub>
                               <m:r>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                 </a:rPr>
                                 <m:t>8</m:t>
@@ -645,25 +649,25 @@
                             </m:sub>
                           </m:sSub>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>𝑀𝑖𝑡𝑖𝑛</m:t>
                           </m:r>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t> </m:t>
                           </m:r>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>𝑃𝑃𝐾</m:t>
                           </m:r>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>+</m:t>
@@ -671,14 +675,14 @@
                           <m:sSub>
                             <m:sSubPr>
                               <m:ctrlPr>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                 </a:rPr>
                               </m:ctrlPr>
                             </m:sSubPr>
                             <m:e>
                               <m:r>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                   <a:ea typeface="Cambria Math" charset="0"/>
                                   <a:cs typeface="Cambria Math" charset="0"/>
@@ -688,7 +692,7 @@
                             </m:e>
                             <m:sub>
                               <m:r>
-                                <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                                <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                                   <a:latin typeface="Cambria Math" charset="0"/>
                                 </a:rPr>
                                 <m:t>9</m:t>
@@ -696,19 +700,19 @@
                             </m:sub>
                           </m:sSub>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>𝐼𝑚𝑝𝑎𝑐𝑡𝑜</m:t>
                           </m:r>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                             </a:rPr>
                             <m:t>+</m:t>
                           </m:r>
                           <m:r>
-                            <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                            <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                               <a:latin typeface="Cambria Math" charset="0"/>
                               <a:ea typeface="Cambria Math" charset="0"/>
                               <a:cs typeface="Cambria Math" charset="0"/>
@@ -720,7 +724,7 @@
                     </m:den>
                   </m:f>
                   <m:r>
-                    <a:rPr lang="es-ES_tradnl" sz="1900" b="0" i="1">
+                    <a:rPr lang="es-ES_tradnl" sz="1800" b="0" i="1">
                       <a:latin typeface="Cambria Math" charset="0"/>
                     </a:rPr>
                     <m:t> </m:t>
@@ -728,14 +732,14 @@
                 </m:oMath>
               </a14:m>
               <a:r>
-                <a:rPr lang="es-ES" sz="2000"/>
+                <a:rPr lang="es-ES" sz="1800"/>
                 <a:t> </a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1"/>
@@ -1222,10 +1226,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R9"/>
+  <dimension ref="A2:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1349,6 +1353,11 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B4:R9"/>

</xml_diff>